<commit_message>
Deploying to gh-pages from @ LinuxForHealth/alvearie-fhir-ig@29b5d72308192f3d5a5ce91c2a110dc2282aade8 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-care-gap-detected-issue.xlsx
+++ b/StructureDefinition-care-gap-detected-issue.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2061" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2061" uniqueCount="362">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-09-07T20:41:11+00:00</t>
+    <t>2022-09-08T16:11:15+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -278,307 +278,311 @@
     <t>Y</t>
   </si>
   <si>
+    <t xml:space="preserve">id
+</t>
+  </si>
+  <si>
+    <t>Logical id of this artifact</t>
+  </si>
+  <si>
+    <t>The logical id of the resource, as used in the URL for the resource. Once assigned, this value never changes.</t>
+  </si>
+  <si>
+    <t>The only time that a resource does not have an id is when it is being submitted to the server using a create operation.</t>
+  </si>
+  <si>
+    <t>Resource.id</t>
+  </si>
+  <si>
+    <t>DetectedIssue.meta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meta {http://ibm.com/fhir/cdm/StructureDefinition/process-meta}
+</t>
+  </si>
+  <si>
+    <t>Metadata about a resource</t>
+  </si>
+  <si>
+    <t>The metadata about a resource. This is content in the resource that is maintained by the infrastructure. Changes to the content might not always be associated with version changes to the resource.</t>
+  </si>
+  <si>
+    <t>Resource.meta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>DetectedIssue.implicitRules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uri
+</t>
+  </si>
+  <si>
+    <t>A set of rules under which this content was created</t>
+  </si>
+  <si>
+    <t>A reference to a set of rules that were followed when the resource was constructed, and which must be understood when processing the content. Often, this is a reference to an implementation guide that defines the special rules along with other profiles etc.</t>
+  </si>
+  <si>
+    <t>Asserting this rule set restricts the content to be only understood by a limited set of trading partners. This inherently limits the usefulness of the data in the long term. However, the existing health eco-system is highly fractured, and not yet ready to define, collect, and exchange data in a generally computable sense. Wherever possible, implementers and/or specification writers should avoid using this element. Often, when used, the URL is a reference to an implementation guide that defines these special rules as part of it's narrative along with other profiles, value sets, etc.</t>
+  </si>
+  <si>
+    <t>Resource.implicitRules</t>
+  </si>
+  <si>
+    <t>DetectedIssue.language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code
+</t>
+  </si>
+  <si>
+    <t>Language of the resource content</t>
+  </si>
+  <si>
+    <t>The base language in which the resource is written.</t>
+  </si>
+  <si>
+    <t>Language is provided to support indexing and accessibility (typically, services such as text to speech use the language tag). The html language tag in the narrative applies  to the narrative. The language tag on the resource may be used to specify the language of other presentations generated from the data in the resource. Not all the content has to be in the base language. The Resource.language should not be assumed to apply to the narrative automatically. If a language is specified, it should it also be specified on the div element in the html (see rules in HTML5 for information about the relationship between xml:lang and the html lang attribute).</t>
+  </si>
+  <si>
+    <t>preferred</t>
+  </si>
+  <si>
+    <t>A human language.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/languages</t>
+  </si>
+  <si>
+    <t>Resource.language</t>
+  </si>
+  <si>
+    <t>DetectedIssue.text</t>
+  </si>
+  <si>
+    <t>narrative
+htmlxhtmldisplay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Narrative
+</t>
+  </si>
+  <si>
+    <t>Text summary of the resource, for human interpretation</t>
+  </si>
+  <si>
+    <t>A human-readable narrative that contains a summary of the resource and can be used to represent the content of the resource to a human. The narrative need not encode all the structured data, but is required to contain sufficient detail to make it "clinically safe" for a human to just read the narrative. Resource definitions may define what content should be represented in the narrative to ensure clinical safety.</t>
+  </si>
+  <si>
+    <t>Contained resources do not have narrative. Resources that are not contained SHOULD have a narrative. In some cases, a resource may only have text with little or no additional discrete data (as long as all minOccurs=1 elements are satisfied).  This may be necessary for data from legacy systems where information is captured as a "text blob" or where text is additionally entered raw or narrated and encoded information is added later.</t>
+  </si>
+  <si>
+    <t>DomainResource.text</t>
+  </si>
+  <si>
+    <t>Act.text?</t>
+  </si>
+  <si>
+    <t>DetectedIssue.contained</t>
+  </si>
+  <si>
+    <t>inline resources
+anonymous resourcescontained resources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource
+</t>
+  </si>
+  <si>
+    <t>Contained, inline Resources</t>
+  </si>
+  <si>
+    <t>These resources do not have an independent existence apart from the resource that contains them - they cannot be identified independently, and nor can they have their own independent transaction scope.</t>
+  </si>
+  <si>
+    <t>This should never be done when the content can be identified properly, as once identification is lost, it is extremely difficult (and context dependent) to restore it again. Contained resources may have profiles and tags In their meta elements, but SHALL NOT have security labels.</t>
+  </si>
+  <si>
+    <t>DomainResource.contained</t>
+  </si>
+  <si>
+    <t>DetectedIssue.extension</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension
+</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>An Extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>DomainResource.extension</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+  </si>
+  <si>
+    <t>canonicalMeasure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://ibm.com/fhir/cdm/StructureDefinition/canonical-measure}
+</t>
+  </si>
+  <si>
+    <t>Canonical reference to the specific version of the measure used to generate the care gap or population</t>
+  </si>
+  <si>
+    <t>measurePopulationId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://ibm.com/fhir/cdm/StructureDefinition/measure-population-id}
+</t>
+  </si>
+  <si>
+    <t>User-friendly textual key (internal use only) that identifies the care gap. This id should be unique across all measures and should not change when a measure is versioned or when overrides are applied.</t>
+  </si>
+  <si>
+    <t>assignedPractitioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://ibm.com/fhir/cdm/StructureDefinition/assigned-practitioner}
+</t>
+  </si>
+  <si>
+    <t>The practitioners assigned to the patient when the care gap or measure population was identified</t>
+  </si>
+  <si>
+    <t>careGapComplianceDisplayName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://ibm.com/fhir/cdm/StructureDefinition/care-gap-compliance-display-name}
+</t>
+  </si>
+  <si>
+    <t>Text describing the treatment or compliance event required to close the care gap.  Should be suitable for display to patient.</t>
+  </si>
+  <si>
+    <t>careGapComplianceFrequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://ibm.com/fhir/cdm/StructureDefinition/care-gap-compliance-frequency}
+</t>
+  </si>
+  <si>
+    <t>Text describing the frequency of the treatment or compliance event required to close the care gap.  Frequency should be suitable for display to patient.</t>
+  </si>
+  <si>
+    <t>careGapComplianceMet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://ibm.com/fhir/cdm/StructureDefinition/care-gap-compliance-met}
+</t>
+  </si>
+  <si>
+    <t>Indicates if the patient received the targeted treatment to close the care gap</t>
+  </si>
+  <si>
+    <t>relatedIssue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://ibm.com/fhir/cdm/StructureDefinition/related-issue}
+</t>
+  </si>
+  <si>
+    <t>Related issue that can be combined to fulfill a single time period for a given care gap</t>
+  </si>
+  <si>
+    <t>DetectedIssue.modifierExtension</t>
+  </si>
+  <si>
+    <t>extensions
+user content</t>
+  </si>
+  <si>
+    <t>Extensions that cannot be ignored</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the resource and that modifies the understanding of the element that contains it and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
+Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
+  </si>
+  <si>
+    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
+  </si>
+  <si>
+    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
+  </si>
+  <si>
+    <t>DomainResource.modifierExtension</t>
+  </si>
+  <si>
+    <t>DetectedIssue.identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifier
+</t>
+  </si>
+  <si>
+    <t>Unique id for the detected issue</t>
+  </si>
+  <si>
+    <t>Business identifier associated with the detected issue record.</t>
+  </si>
+  <si>
+    <t>Allows linking instances of the same detected issue found on different servers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:type}
+</t>
+  </si>
+  <si>
+    <t>Slice based on entry system</t>
+  </si>
+  <si>
+    <t>Event.identifier</t>
+  </si>
+  <si>
+    <t>IAM-7</t>
+  </si>
+  <si>
+    <t>.id</t>
+  </si>
+  <si>
+    <t>FiveWs.identifier</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>DetectedIssue.identifier.id</t>
+  </si>
+  <si>
     <t xml:space="preserve">string
 </t>
-  </si>
-  <si>
-    <t>Logical id of this artifact</t>
-  </si>
-  <si>
-    <t>The logical id of the resource, as used in the URL for the resource. Once assigned, this value never changes.</t>
-  </si>
-  <si>
-    <t>The only time that a resource does not have an id is when it is being submitted to the server using a create operation.</t>
-  </si>
-  <si>
-    <t>Resource.id</t>
-  </si>
-  <si>
-    <t>DetectedIssue.meta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meta {http://ibm.com/fhir/cdm/StructureDefinition/process-meta}
-</t>
-  </si>
-  <si>
-    <t>Metadata about a resource</t>
-  </si>
-  <si>
-    <t>The metadata about a resource. This is content in the resource that is maintained by the infrastructure. Changes to the content might not always be associated with version changes to the resource.</t>
-  </si>
-  <si>
-    <t>Resource.meta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ele-1
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>DetectedIssue.implicitRules</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uri
-</t>
-  </si>
-  <si>
-    <t>A set of rules under which this content was created</t>
-  </si>
-  <si>
-    <t>A reference to a set of rules that were followed when the resource was constructed, and which must be understood when processing the content. Often, this is a reference to an implementation guide that defines the special rules along with other profiles etc.</t>
-  </si>
-  <si>
-    <t>Asserting this rule set restricts the content to be only understood by a limited set of trading partners. This inherently limits the usefulness of the data in the long term. However, the existing health eco-system is highly fractured, and not yet ready to define, collect, and exchange data in a generally computable sense. Wherever possible, implementers and/or specification writers should avoid using this element. Often, when used, the URL is a reference to an implementation guide that defines these special rules as part of it's narrative along with other profiles, value sets, etc.</t>
-  </si>
-  <si>
-    <t>Resource.implicitRules</t>
-  </si>
-  <si>
-    <t>DetectedIssue.language</t>
-  </si>
-  <si>
-    <t xml:space="preserve">code
-</t>
-  </si>
-  <si>
-    <t>Language of the resource content</t>
-  </si>
-  <si>
-    <t>The base language in which the resource is written.</t>
-  </si>
-  <si>
-    <t>Language is provided to support indexing and accessibility (typically, services such as text to speech use the language tag). The html language tag in the narrative applies  to the narrative. The language tag on the resource may be used to specify the language of other presentations generated from the data in the resource. Not all the content has to be in the base language. The Resource.language should not be assumed to apply to the narrative automatically. If a language is specified, it should it also be specified on the div element in the html (see rules in HTML5 for information about the relationship between xml:lang and the html lang attribute).</t>
-  </si>
-  <si>
-    <t>preferred</t>
-  </si>
-  <si>
-    <t>A human language.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/languages</t>
-  </si>
-  <si>
-    <t>Resource.language</t>
-  </si>
-  <si>
-    <t>DetectedIssue.text</t>
-  </si>
-  <si>
-    <t>narrative
-htmlxhtmldisplay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Narrative
-</t>
-  </si>
-  <si>
-    <t>Text summary of the resource, for human interpretation</t>
-  </si>
-  <si>
-    <t>A human-readable narrative that contains a summary of the resource and can be used to represent the content of the resource to a human. The narrative need not encode all the structured data, but is required to contain sufficient detail to make it "clinically safe" for a human to just read the narrative. Resource definitions may define what content should be represented in the narrative to ensure clinical safety.</t>
-  </si>
-  <si>
-    <t>Contained resources do not have narrative. Resources that are not contained SHOULD have a narrative. In some cases, a resource may only have text with little or no additional discrete data (as long as all minOccurs=1 elements are satisfied).  This may be necessary for data from legacy systems where information is captured as a "text blob" or where text is additionally entered raw or narrated and encoded information is added later.</t>
-  </si>
-  <si>
-    <t>DomainResource.text</t>
-  </si>
-  <si>
-    <t>Act.text?</t>
-  </si>
-  <si>
-    <t>DetectedIssue.contained</t>
-  </si>
-  <si>
-    <t>inline resources
-anonymous resourcescontained resources</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource
-</t>
-  </si>
-  <si>
-    <t>Contained, inline Resources</t>
-  </si>
-  <si>
-    <t>These resources do not have an independent existence apart from the resource that contains them - they cannot be identified independently, and nor can they have their own independent transaction scope.</t>
-  </si>
-  <si>
-    <t>This should never be done when the content can be identified properly, as once identification is lost, it is extremely difficult (and context dependent) to restore it again. Contained resources may have profiles and tags In their meta elements, but SHALL NOT have security labels.</t>
-  </si>
-  <si>
-    <t>DomainResource.contained</t>
-  </si>
-  <si>
-    <t>DetectedIssue.extension</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension
-</t>
-  </si>
-  <si>
-    <t>Extension</t>
-  </si>
-  <si>
-    <t>An Extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>DomainResource.extension</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
-  </si>
-  <si>
-    <t>canonicalMeasure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {http://ibm.com/fhir/cdm/StructureDefinition/canonical-measure}
-</t>
-  </si>
-  <si>
-    <t>Canonical reference to the specific version of the measure used to generate the care gap or population</t>
-  </si>
-  <si>
-    <t>measurePopulationId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {http://ibm.com/fhir/cdm/StructureDefinition/measure-population-id}
-</t>
-  </si>
-  <si>
-    <t>User-friendly textual key (internal use only) that identifies the care gap. This id should be unique across all measures and should not change when a measure is versioned or when overrides are applied.</t>
-  </si>
-  <si>
-    <t>assignedPractitioner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {http://ibm.com/fhir/cdm/StructureDefinition/assigned-practitioner}
-</t>
-  </si>
-  <si>
-    <t>The practitioners assigned to the patient when the care gap or measure population was identified</t>
-  </si>
-  <si>
-    <t>careGapComplianceDisplayName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {http://ibm.com/fhir/cdm/StructureDefinition/care-gap-compliance-display-name}
-</t>
-  </si>
-  <si>
-    <t>Text describing the treatment or compliance event required to close the care gap.  Should be suitable for display to patient.</t>
-  </si>
-  <si>
-    <t>careGapComplianceFrequency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {http://ibm.com/fhir/cdm/StructureDefinition/care-gap-compliance-frequency}
-</t>
-  </si>
-  <si>
-    <t>Text describing the frequency of the treatment or compliance event required to close the care gap.  Frequency should be suitable for display to patient.</t>
-  </si>
-  <si>
-    <t>careGapComplianceMet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {http://ibm.com/fhir/cdm/StructureDefinition/care-gap-compliance-met}
-</t>
-  </si>
-  <si>
-    <t>Indicates if the patient received the targeted treatment to close the care gap</t>
-  </si>
-  <si>
-    <t>relatedIssue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {http://ibm.com/fhir/cdm/StructureDefinition/related-issue}
-</t>
-  </si>
-  <si>
-    <t>Related issue that can be combined to fulfill a single time period for a given care gap</t>
-  </si>
-  <si>
-    <t>DetectedIssue.modifierExtension</t>
-  </si>
-  <si>
-    <t>extensions
-user content</t>
-  </si>
-  <si>
-    <t>Extensions that cannot be ignored</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the resource and that modifies the understanding of the element that contains it and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
-Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
-  </si>
-  <si>
-    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
-  </si>
-  <si>
-    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
-  </si>
-  <si>
-    <t>DomainResource.modifierExtension</t>
-  </si>
-  <si>
-    <t>DetectedIssue.identifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identifier
-</t>
-  </si>
-  <si>
-    <t>Unique id for the detected issue</t>
-  </si>
-  <si>
-    <t>Business identifier associated with the detected issue record.</t>
-  </si>
-  <si>
-    <t>Allows linking instances of the same detected issue found on different servers.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:type}
-</t>
-  </si>
-  <si>
-    <t>Slice based on entry system</t>
-  </si>
-  <si>
-    <t>Event.identifier</t>
-  </si>
-  <si>
-    <t>IAM-7</t>
-  </si>
-  <si>
-    <t>.id</t>
-  </si>
-  <si>
-    <t>FiveWs.identifier</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>DetectedIssue.identifier.id</t>
   </si>
   <si>
     <t>Unique id for inter-element referencing</t>
@@ -3631,13 +3635,13 @@
         <v>77</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>87</v>
+        <v>180</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -3688,7 +3692,7 @@
         <v>77</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>75</v>
@@ -3709,7 +3713,7 @@
         <v>77</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AM20" t="s" s="2">
         <v>77</v>
@@ -3717,7 +3721,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3743,10 +3747,10 @@
         <v>132</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M21" t="s" s="2">
         <v>164</v>
@@ -3790,7 +3794,7 @@
         <v>135</v>
       </c>
       <c r="AB21" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AC21" t="s" s="2">
         <v>77</v>
@@ -3799,7 +3803,7 @@
         <v>136</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>75</v>
@@ -3820,7 +3824,7 @@
         <v>77</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AM21" t="s" s="2">
         <v>77</v>
@@ -3828,7 +3832,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3854,16 +3858,16 @@
         <v>107</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>77</v>
@@ -3873,7 +3877,7 @@
         <v>77</v>
       </c>
       <c r="R22" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="S22" t="s" s="2">
         <v>77</v>
@@ -3888,13 +3892,13 @@
         <v>77</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="X22" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="Y22" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>77</v>
@@ -3912,7 +3916,7 @@
         <v>77</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>75</v>
@@ -3933,7 +3937,7 @@
         <v>99</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AM22" t="s" s="2">
         <v>77</v>
@@ -3941,7 +3945,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3964,19 +3968,19 @@
         <v>86</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>77</v>
@@ -3986,7 +3990,7 @@
         <v>77</v>
       </c>
       <c r="R23" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="S23" t="s" s="2">
         <v>77</v>
@@ -4001,13 +4005,13 @@
         <v>77</v>
       </c>
       <c r="W23" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>77</v>
@@ -4025,7 +4029,7 @@
         <v>77</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>75</v>
@@ -4043,10 +4047,10 @@
         <v>77</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AM23" t="s" s="2">
         <v>77</v>
@@ -4054,7 +4058,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4080,16 +4084,16 @@
         <v>101</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>77</v>
@@ -4102,7 +4106,7 @@
         <v>77</v>
       </c>
       <c r="S24" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="T24" t="s" s="2">
         <v>77</v>
@@ -4138,7 +4142,7 @@
         <v>77</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>75</v>
@@ -4156,10 +4160,10 @@
         <v>77</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AM24" t="s" s="2">
         <v>77</v>
@@ -4167,7 +4171,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4190,16 +4194,16 @@
         <v>86</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>87</v>
+        <v>180</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
@@ -4213,7 +4217,7 @@
         <v>77</v>
       </c>
       <c r="S25" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="T25" t="s" s="2">
         <v>77</v>
@@ -4249,7 +4253,7 @@
         <v>77</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>75</v>
@@ -4267,10 +4271,10 @@
         <v>77</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AM25" t="s" s="2">
         <v>77</v>
@@ -4278,7 +4282,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4301,13 +4305,13 @@
         <v>86</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -4358,7 +4362,7 @@
         <v>77</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>75</v>
@@ -4376,10 +4380,10 @@
         <v>77</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AM26" t="s" s="2">
         <v>77</v>
@@ -4387,7 +4391,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4410,16 +4414,16 @@
         <v>86</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
@@ -4469,7 +4473,7 @@
         <v>77</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>75</v>
@@ -4487,10 +4491,10 @@
         <v>77</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AM27" t="s" s="2">
         <v>77</v>
@@ -4501,7 +4505,7 @@
         <v>167</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C28" t="s" s="2">
         <v>77</v>
@@ -4634,13 +4638,13 @@
         <v>77</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>87</v>
+        <v>180</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -4691,7 +4695,7 @@
         <v>77</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>75</v>
@@ -4712,7 +4716,7 @@
         <v>77</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AM29" t="s" s="2">
         <v>77</v>
@@ -4720,7 +4724,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4746,10 +4750,10 @@
         <v>132</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M30" t="s" s="2">
         <v>164</v>
@@ -4793,7 +4797,7 @@
         <v>135</v>
       </c>
       <c r="AB30" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AC30" t="s" s="2">
         <v>77</v>
@@ -4802,7 +4806,7 @@
         <v>136</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>75</v>
@@ -4823,7 +4827,7 @@
         <v>77</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AM30" t="s" s="2">
         <v>77</v>
@@ -4831,7 +4835,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4857,16 +4861,16 @@
         <v>107</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="O31" t="s" s="2">
         <v>77</v>
@@ -4876,7 +4880,7 @@
         <v>77</v>
       </c>
       <c r="R31" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="S31" t="s" s="2">
         <v>77</v>
@@ -4891,13 +4895,13 @@
         <v>77</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="Z31" t="s" s="2">
         <v>77</v>
@@ -4915,7 +4919,7 @@
         <v>77</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>75</v>
@@ -4936,7 +4940,7 @@
         <v>99</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AM31" t="s" s="2">
         <v>77</v>
@@ -4944,7 +4948,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4967,19 +4971,19 @@
         <v>86</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>77</v>
@@ -4989,7 +4993,7 @@
         <v>77</v>
       </c>
       <c r="R32" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="S32" t="s" s="2">
         <v>77</v>
@@ -5004,13 +5008,13 @@
         <v>77</v>
       </c>
       <c r="W32" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="X32" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Y32" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="Z32" t="s" s="2">
         <v>77</v>
@@ -5028,7 +5032,7 @@
         <v>77</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>75</v>
@@ -5046,10 +5050,10 @@
         <v>77</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AM32" t="s" s="2">
         <v>77</v>
@@ -5057,7 +5061,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5083,16 +5087,16 @@
         <v>101</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>77</v>
@@ -5105,7 +5109,7 @@
         <v>77</v>
       </c>
       <c r="S33" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="T33" t="s" s="2">
         <v>77</v>
@@ -5141,7 +5145,7 @@
         <v>77</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>75</v>
@@ -5159,10 +5163,10 @@
         <v>77</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AM33" t="s" s="2">
         <v>77</v>
@@ -5170,7 +5174,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5193,16 +5197,16 @@
         <v>86</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>87</v>
+        <v>180</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
@@ -5216,7 +5220,7 @@
         <v>77</v>
       </c>
       <c r="S34" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="T34" t="s" s="2">
         <v>77</v>
@@ -5252,7 +5256,7 @@
         <v>77</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>75</v>
@@ -5270,10 +5274,10 @@
         <v>77</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>77</v>
@@ -5281,7 +5285,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5304,13 +5308,13 @@
         <v>86</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5361,7 +5365,7 @@
         <v>77</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>75</v>
@@ -5379,10 +5383,10 @@
         <v>77</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AM35" t="s" s="2">
         <v>77</v>
@@ -5390,7 +5394,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5413,16 +5417,16 @@
         <v>86</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
@@ -5472,7 +5476,7 @@
         <v>77</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>75</v>
@@ -5490,10 +5494,10 @@
         <v>77</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AM36" t="s" s="2">
         <v>77</v>
@@ -5501,11 +5505,11 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
@@ -5527,13 +5531,13 @@
         <v>107</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
@@ -5559,13 +5563,13 @@
         <v>77</v>
       </c>
       <c r="W37" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>77</v>
@@ -5583,7 +5587,7 @@
         <v>77</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>85</v>
@@ -5598,7 +5602,7 @@
         <v>98</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>77</v>
@@ -5607,16 +5611,16 @@
         <v>77</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" t="s" s="2">
@@ -5635,13 +5639,13 @@
         <v>86</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5671,10 +5675,10 @@
         <v>111</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>77</v>
@@ -5692,7 +5696,7 @@
         <v>77</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>75</v>
@@ -5707,25 +5711,25 @@
         <v>98</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
@@ -5747,10 +5751,10 @@
         <v>107</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -5777,13 +5781,13 @@
         <v>77</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>77</v>
@@ -5801,7 +5805,7 @@
         <v>77</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>75</v>
@@ -5819,18 +5823,18 @@
         <v>77</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5853,17 +5857,17 @@
         <v>86</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>77</v>
@@ -5912,7 +5916,7 @@
         <v>77</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>75</v>
@@ -5927,21 +5931,21 @@
         <v>98</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5964,17 +5968,17 @@
         <v>86</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>77</v>
@@ -6023,7 +6027,7 @@
         <v>77</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>75</v>
@@ -6038,21 +6042,21 @@
         <v>98</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6075,13 +6079,13 @@
         <v>86</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -6132,7 +6136,7 @@
         <v>77</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>75</v>
@@ -6147,25 +6151,25 @@
         <v>98</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
@@ -6184,16 +6188,16 @@
         <v>86</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
@@ -6243,7 +6247,7 @@
         <v>77</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>75</v>
@@ -6258,13 +6262,13 @@
         <v>98</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AM43" t="s" s="2">
         <v>77</v>
@@ -6272,7 +6276,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6295,13 +6299,13 @@
         <v>77</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6352,7 +6356,7 @@
         <v>77</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>75</v>
@@ -6376,12 +6380,12 @@
         <v>77</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6404,13 +6408,13 @@
         <v>77</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>87</v>
+        <v>180</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -6461,7 +6465,7 @@
         <v>77</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>75</v>
@@ -6482,7 +6486,7 @@
         <v>77</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AM45" t="s" s="2">
         <v>77</v>
@@ -6490,7 +6494,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6516,10 +6520,10 @@
         <v>132</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M46" t="s" s="2">
         <v>164</v>
@@ -6572,7 +6576,7 @@
         <v>77</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>75</v>
@@ -6593,7 +6597,7 @@
         <v>77</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AM46" t="s" s="2">
         <v>77</v>
@@ -6601,11 +6605,11 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
@@ -6627,10 +6631,10 @@
         <v>132</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="M47" t="s" s="2">
         <v>164</v>
@@ -6685,7 +6689,7 @@
         <v>77</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>75</v>
@@ -6714,7 +6718,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6737,13 +6741,13 @@
         <v>77</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -6770,13 +6774,13 @@
         <v>77</v>
       </c>
       <c r="W48" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>77</v>
@@ -6794,7 +6798,7 @@
         <v>77</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>75</v>
@@ -6818,12 +6822,12 @@
         <v>77</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6846,13 +6850,13 @@
         <v>77</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -6903,7 +6907,7 @@
         <v>77</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>75</v>
@@ -6927,12 +6931,12 @@
         <v>77</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6955,16 +6959,16 @@
         <v>77</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>87</v>
+        <v>180</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
@@ -7014,7 +7018,7 @@
         <v>77</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>75</v>
@@ -7029,13 +7033,13 @@
         <v>98</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AM50" t="s" s="2">
         <v>77</v>
@@ -7043,7 +7047,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7069,10 +7073,10 @@
         <v>101</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -7123,7 +7127,7 @@
         <v>77</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>75</v>
@@ -7144,7 +7148,7 @@
         <v>77</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="AM51" t="s" s="2">
         <v>77</v>
@@ -7152,7 +7156,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7175,13 +7179,13 @@
         <v>77</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
@@ -7232,7 +7236,7 @@
         <v>77</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>75</v>
@@ -7253,7 +7257,7 @@
         <v>77</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AM52" t="s" s="2">
         <v>77</v>
@@ -7261,7 +7265,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7284,13 +7288,13 @@
         <v>77</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>87</v>
+        <v>180</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -7341,7 +7345,7 @@
         <v>77</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>75</v>
@@ -7362,7 +7366,7 @@
         <v>77</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AM53" t="s" s="2">
         <v>77</v>
@@ -7370,7 +7374,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7396,10 +7400,10 @@
         <v>132</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M54" t="s" s="2">
         <v>164</v>
@@ -7452,7 +7456,7 @@
         <v>77</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>75</v>
@@ -7473,7 +7477,7 @@
         <v>77</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AM54" t="s" s="2">
         <v>77</v>
@@ -7481,11 +7485,11 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
@@ -7507,10 +7511,10 @@
         <v>132</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="M55" t="s" s="2">
         <v>164</v>
@@ -7565,7 +7569,7 @@
         <v>77</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>75</v>
@@ -7594,7 +7598,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7617,16 +7621,16 @@
         <v>77</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" t="s" s="2">
@@ -7655,10 +7659,10 @@
         <v>111</v>
       </c>
       <c r="X56" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="Y56" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="Z56" t="s" s="2">
         <v>77</v>
@@ -7676,7 +7680,7 @@
         <v>77</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>85</v>
@@ -7697,7 +7701,7 @@
         <v>77</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AM56" t="s" s="2">
         <v>77</v>
@@ -7705,7 +7709,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7728,16 +7732,16 @@
         <v>77</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" t="s" s="2">
@@ -7787,7 +7791,7 @@
         <v>77</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>75</v>
@@ -7808,7 +7812,7 @@
         <v>77</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AM57" t="s" s="2">
         <v>77</v>
@@ -7816,7 +7820,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7839,13 +7843,13 @@
         <v>77</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -7896,7 +7900,7 @@
         <v>77</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>75</v>
@@ -7917,7 +7921,7 @@
         <v>77</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AM58" t="s" s="2">
         <v>77</v>

</xml_diff>